<commit_message>
final touches and validation for rev B
</commit_message>
<xml_diff>
--- a/EAGLE/vr61/vr61-dims.xlsx
+++ b/EAGLE/vr61/vr61-dims.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vino/dev/tecsmith/vr61-keyboard-pcb/EAGLE/vr61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149A3D07-2D84-044C-BA50-C884A9D44DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA80EA6E-50F0-1841-94FD-C3FA5D76AB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{0C56D587-A2A5-2845-B156-89675C65F849}"/>
   </bookViews>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3CEA42-800C-9F4D-A1A4-CF3E8C4B5B18}">
   <dimension ref="B1:W57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53:O57"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10:W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,11 +769,11 @@
         <v>19.05</v>
       </c>
       <c r="V4">
-        <f>S4*Q4</f>
+        <f>(S4*Q4)</f>
         <v>285.75</v>
       </c>
       <c r="W4">
-        <f>S4*COUNT(Q2:Q6)</f>
+        <f>(S4*COUNT(Q2:Q6))</f>
         <v>95.25</v>
       </c>
     </row>
@@ -906,117 +906,117 @@
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B9">
-        <f>B2*$S$4</f>
+        <f t="shared" ref="B9:O9" si="0">B2*$S$4</f>
         <v>19.05</v>
       </c>
       <c r="C9">
-        <f>C2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="D9">
-        <f>D2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="E9">
-        <f>E2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="F9">
-        <f>F2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="G9">
-        <f>G2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="H9">
-        <f>H2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="I9">
-        <f>I2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="J9">
-        <f>J2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="K9">
-        <f>K2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="L9">
-        <f>L2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="M9">
-        <f>M2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="N9">
-        <f>N2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>19.05</v>
       </c>
       <c r="O9">
-        <f>O2*$S$4</f>
+        <f t="shared" si="0"/>
         <v>38.1</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B10">
-        <f>B3*$S$4</f>
+        <f t="shared" ref="B10:O10" si="1">B3*$S$4</f>
         <v>28.575000000000003</v>
       </c>
       <c r="C10">
-        <f>C3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="D10">
-        <f>D3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="E10">
-        <f>E3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="F10">
-        <f>F3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="G10">
-        <f>G3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="H10">
-        <f>H3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="I10">
-        <f>I3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="J10">
-        <f>J3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="K10">
-        <f>K3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="L10">
-        <f>L3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="M10">
-        <f>M3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="N10">
-        <f>N3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>19.05</v>
       </c>
       <c r="O10">
-        <f>O3*$S$4</f>
+        <f t="shared" si="1"/>
         <v>28.575000000000003</v>
       </c>
       <c r="U10" t="str">
@@ -1030,117 +1030,117 @@
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B11">
-        <f>B4*$S$4</f>
+        <f t="shared" ref="B11:O11" si="2">B4*$S$4</f>
         <v>33.337499999999999</v>
       </c>
       <c r="C11">
-        <f>C4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
       <c r="D11">
-        <f>D4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
       <c r="E11">
-        <f>E4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
       <c r="F11">
-        <f>F4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
       <c r="G11">
-        <f>G4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
       <c r="H11">
-        <f>H4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
       <c r="I11">
-        <f>I4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
       <c r="J11">
-        <f>J4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
       <c r="K11">
-        <f>K4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
       <c r="L11">
-        <f>L4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
       <c r="M11">
-        <f>M4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>19.05</v>
       </c>
       <c r="N11" s="1">
-        <f>N4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O11">
-        <f>O4*$S$4</f>
+        <f t="shared" si="2"/>
         <v>42.862500000000004</v>
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B12">
-        <f>B5*$S$4</f>
+        <f t="shared" ref="B12:O12" si="3">B5*$S$4</f>
         <v>42.862500000000004</v>
       </c>
       <c r="C12" s="1">
-        <f>C5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D12">
-        <f>D5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>19.05</v>
       </c>
       <c r="E12">
-        <f>E5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>19.05</v>
       </c>
       <c r="F12">
-        <f>F5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>19.05</v>
       </c>
       <c r="G12">
-        <f>G5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>19.05</v>
       </c>
       <c r="H12">
-        <f>H5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>19.05</v>
       </c>
       <c r="I12">
-        <f>I5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>19.05</v>
       </c>
       <c r="J12">
-        <f>J5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>19.05</v>
       </c>
       <c r="K12">
-        <f>K5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>19.05</v>
       </c>
       <c r="L12">
-        <f>L5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>19.05</v>
       </c>
       <c r="M12">
-        <f>M5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>19.05</v>
       </c>
       <c r="N12" s="1">
-        <f>N5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O12">
-        <f>O5*$S$4</f>
+        <f t="shared" si="3"/>
         <v>52.387500000000003</v>
       </c>
     </row>
@@ -1154,51 +1154,51 @@
         <v>23.8125</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:O13" si="0">D6*$S$4</f>
+        <f t="shared" ref="D13:O13" si="4">D6*$S$4</f>
         <v>23.8125</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.0625</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>23.8125</v>
       </c>
       <c r="M13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>23.8125</v>
       </c>
       <c r="N13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>23.8125</v>
       </c>
       <c r="O13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>23.8125</v>
       </c>
     </row>
@@ -1225,51 +1225,51 @@
         <v>38.1</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16:O16" si="1">D9+C16</f>
+        <f t="shared" ref="D16:O16" si="5">D9+C16</f>
         <v>57.150000000000006</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>76.2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>95.25</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>114.3</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>133.35</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>152.4</v>
       </c>
       <c r="J16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>171.45000000000002</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>190.50000000000003</v>
       </c>
       <c r="L16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>209.55000000000004</v>
       </c>
       <c r="M16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>228.60000000000005</v>
       </c>
       <c r="N16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>247.65000000000006</v>
       </c>
       <c r="O16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>285.75000000000006</v>
       </c>
     </row>
@@ -1283,51 +1283,51 @@
         <v>47.625</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:O17" si="2">D10+C17</f>
+        <f t="shared" ref="D17:O17" si="6">D10+C17</f>
         <v>66.674999999999997</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>85.724999999999994</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>104.77499999999999</v>
       </c>
       <c r="G17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>123.82499999999999</v>
       </c>
       <c r="H17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>142.875</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>161.92500000000001</v>
       </c>
       <c r="J17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>180.97500000000002</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>200.02500000000003</v>
       </c>
       <c r="L17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>219.07500000000005</v>
       </c>
       <c r="M17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>238.12500000000006</v>
       </c>
       <c r="N17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>257.17500000000007</v>
       </c>
       <c r="O17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>285.75000000000006</v>
       </c>
     </row>
@@ -1341,51 +1341,51 @@
         <v>52.387500000000003</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:O18" si="3">D11+C18</f>
+        <f t="shared" ref="D18:O18" si="7">D11+C18</f>
         <v>71.4375</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>90.487499999999997</v>
       </c>
       <c r="F18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>109.53749999999999</v>
       </c>
       <c r="G18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>128.58750000000001</v>
       </c>
       <c r="H18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>147.63750000000002</v>
       </c>
       <c r="I18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>166.68750000000003</v>
       </c>
       <c r="J18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>185.73750000000004</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>204.78750000000005</v>
       </c>
       <c r="L18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>223.83750000000006</v>
       </c>
       <c r="M18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>242.88750000000007</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>242.88750000000007</v>
       </c>
       <c r="O18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>285.75000000000006</v>
       </c>
     </row>
@@ -1399,51 +1399,51 @@
         <v>42.862500000000004</v>
       </c>
       <c r="D19">
-        <f t="shared" ref="D19:O19" si="4">D12+C19</f>
+        <f t="shared" ref="D19:O19" si="8">D12+C19</f>
         <v>61.912500000000009</v>
       </c>
       <c r="E19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>80.962500000000006</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>100.0125</v>
       </c>
       <c r="G19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>119.0625</v>
       </c>
       <c r="H19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>138.11250000000001</v>
       </c>
       <c r="I19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>157.16250000000002</v>
       </c>
       <c r="J19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>176.21250000000003</v>
       </c>
       <c r="K19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>195.26250000000005</v>
       </c>
       <c r="L19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>214.31250000000006</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>233.36250000000007</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>233.36250000000007</v>
       </c>
       <c r="O19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>285.75000000000006</v>
       </c>
     </row>
@@ -1457,51 +1457,51 @@
         <v>47.625</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20:O20" si="5">D13+C20</f>
+        <f t="shared" ref="D20:O20" si="9">D13+C20</f>
         <v>71.4375</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>71.4375</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>71.4375</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>71.4375</v>
       </c>
       <c r="H20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>190.5</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>190.5</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>190.5</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>190.5</v>
       </c>
       <c r="L20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>214.3125</v>
       </c>
       <c r="M20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>238.125</v>
       </c>
       <c r="N20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>261.9375</v>
       </c>
       <c r="O20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>285.75</v>
       </c>
     </row>
@@ -1516,55 +1516,55 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:O23" si="6">ROUND(C16-(C9/2), 3)</f>
+        <f t="shared" ref="C23:O23" si="10">ROUND(C16-(C9/2), 3)</f>
         <v>28.574999999999999</v>
       </c>
       <c r="D23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>47.625</v>
       </c>
       <c r="E23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>66.674999999999997</v>
       </c>
       <c r="F23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>85.724999999999994</v>
       </c>
       <c r="G23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>104.77500000000001</v>
       </c>
       <c r="H23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>123.825</v>
       </c>
       <c r="I23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>142.875</v>
       </c>
       <c r="J23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>161.92500000000001</v>
       </c>
       <c r="K23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>180.97499999999999</v>
       </c>
       <c r="L23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>200.02500000000001</v>
       </c>
       <c r="M23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>219.07499999999999</v>
       </c>
       <c r="N23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>238.125</v>
       </c>
       <c r="O23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>266.7</v>
       </c>
       <c r="Q23">
@@ -1574,59 +1574,59 @@
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24">
-        <f t="shared" ref="B24:O24" si="7">ROUND(B17-(B10/2), 3)</f>
+        <f t="shared" ref="B24:O24" si="11">ROUND(B17-(B10/2), 3)</f>
         <v>14.288</v>
       </c>
       <c r="C24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>38.1</v>
       </c>
       <c r="D24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>57.15</v>
       </c>
       <c r="E24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>76.2</v>
       </c>
       <c r="F24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>95.25</v>
       </c>
       <c r="G24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>114.3</v>
       </c>
       <c r="H24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>133.35</v>
       </c>
       <c r="I24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>152.4</v>
       </c>
       <c r="J24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>171.45</v>
       </c>
       <c r="K24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>190.5</v>
       </c>
       <c r="L24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>209.55</v>
       </c>
       <c r="M24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>228.6</v>
       </c>
       <c r="N24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>247.65</v>
       </c>
       <c r="O24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>271.46300000000002</v>
       </c>
       <c r="Q24">
@@ -1636,7 +1636,7 @@
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25">
-        <f t="shared" ref="B25:M25" si="8">ROUND(B18-(B11/2), 3)</f>
+        <f t="shared" ref="B25:M25" si="12">ROUND(B18-(B11/2), 3)</f>
         <v>16.669</v>
       </c>
       <c r="C25">
@@ -1644,48 +1644,48 @@
         <v>42.863</v>
       </c>
       <c r="D25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>61.912999999999997</v>
       </c>
       <c r="E25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>80.962999999999994</v>
       </c>
       <c r="F25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>100.01300000000001</v>
       </c>
       <c r="G25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>119.063</v>
       </c>
       <c r="H25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>138.113</v>
       </c>
       <c r="I25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>157.16300000000001</v>
       </c>
       <c r="J25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>176.21299999999999</v>
       </c>
       <c r="K25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>195.26300000000001</v>
       </c>
       <c r="L25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>214.31299999999999</v>
       </c>
       <c r="M25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>233.363</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25">
-        <f t="shared" ref="O25:O26" si="9">ROUND(O18-(O11/2), 3)</f>
+        <f t="shared" ref="O25:O26" si="13">ROUND(O18-(O11/2), 3)</f>
         <v>264.31900000000002</v>
       </c>
       <c r="Q25">
@@ -1700,48 +1700,48 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26">
-        <f t="shared" ref="D26:M26" si="10">ROUND(D19-(D12/2), 3)</f>
+        <f t="shared" ref="D26:M26" si="14">ROUND(D19-(D12/2), 3)</f>
         <v>52.387999999999998</v>
       </c>
       <c r="E26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>71.438000000000002</v>
       </c>
       <c r="F26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>90.488</v>
       </c>
       <c r="G26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>109.538</v>
       </c>
       <c r="H26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>128.58799999999999</v>
       </c>
       <c r="I26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>147.63800000000001</v>
       </c>
       <c r="J26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>166.68799999999999</v>
       </c>
       <c r="K26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>185.738</v>
       </c>
       <c r="L26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>204.78800000000001</v>
       </c>
       <c r="M26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>223.83799999999999</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>259.55599999999998</v>
       </c>
       <c r="Q26">
@@ -1751,15 +1751,15 @@
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27">
-        <f t="shared" ref="B27:D27" si="11">ROUND(B20-(B13/2), 3)</f>
+        <f t="shared" ref="B27:D27" si="15">ROUND(B20-(B13/2), 3)</f>
         <v>11.906000000000001</v>
       </c>
       <c r="C27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>35.719000000000001</v>
       </c>
       <c r="D27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>59.530999999999999</v>
       </c>
       <c r="E27" s="1"/>
@@ -1773,19 +1773,19 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27">
-        <f t="shared" ref="L27:O27" si="12">ROUND(L20-(L13/2), 3)</f>
+        <f t="shared" ref="L27:O27" si="16">ROUND(L20-(L13/2), 3)</f>
         <v>202.40600000000001</v>
       </c>
       <c r="M27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>226.21899999999999</v>
       </c>
       <c r="N27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>250.03100000000001</v>
       </c>
       <c r="O27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>273.84399999999999</v>
       </c>
       <c r="Q27">
@@ -2002,55 +2002,55 @@
         <v xml:space="preserve">MOVE S_ESC (9.525 85.725); </v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" ref="C37:O37" si="13">_xlfn.CONCAT("MOVE S_", C30, " (", C23, " ", $Q23,"); ")</f>
+        <f t="shared" ref="C37:O37" si="17">_xlfn.CONCAT("MOVE S_", C30, " (", C23, " ", $Q23,"); ")</f>
         <v xml:space="preserve">MOVE S_1 (28.575 85.725); </v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_2 (47.625 85.725); </v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_3 (66.675 85.725); </v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_4 (85.725 85.725); </v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_5 (104.775 85.725); </v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_6 (123.825 85.725); </v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_7 (142.875 85.725); </v>
       </c>
       <c r="J37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_8 (161.925 85.725); </v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_9 (180.975 85.725); </v>
       </c>
       <c r="L37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_0 (200.025 85.725); </v>
       </c>
       <c r="M37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_MINS (219.075 85.725); </v>
       </c>
       <c r="N37" s="4" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_EQL (238.125 85.725); </v>
       </c>
       <c r="O37" s="2" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">MOVE S_BSPC (266.7 85.725); </v>
       </c>
     </row>
@@ -2060,55 +2060,55 @@
         <v xml:space="preserve">MOVE S_TAB (14.288 66.675); </v>
       </c>
       <c r="C38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", C31, " (", C24, " ", $Q24,"); ")</f>
+        <f t="shared" ref="C38:O38" si="18">_xlfn.CONCAT("MOVE S_", C31, " (", C24, " ", $Q24,"); ")</f>
         <v xml:space="preserve">MOVE S_Q (38.1 66.675); </v>
       </c>
       <c r="D38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", D31, " (", D24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_W (57.15 66.675); </v>
       </c>
       <c r="E38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", E31, " (", E24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_E (76.2 66.675); </v>
       </c>
       <c r="F38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", F31, " (", F24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_R (95.25 66.675); </v>
       </c>
       <c r="G38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", G31, " (", G24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_T (114.3 66.675); </v>
       </c>
       <c r="H38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", H31, " (", H24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_Y (133.35 66.675); </v>
       </c>
       <c r="I38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", I31, " (", I24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_U (152.4 66.675); </v>
       </c>
       <c r="J38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", J31, " (", J24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_I (171.45 66.675); </v>
       </c>
       <c r="K38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", K31, " (", K24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_O (190.5 66.675); </v>
       </c>
       <c r="L38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", L31, " (", L24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_P (209.55 66.675); </v>
       </c>
       <c r="M38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", M31, " (", M24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_LBRC (228.6 66.675); </v>
       </c>
       <c r="N38" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", N31, " (", N24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_RBRC (247.65 66.675); </v>
       </c>
       <c r="O38" s="4" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", O31, " (", O24, " ", $Q24,"); ")</f>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">MOVE S_BSLS (271.463 66.675); </v>
       </c>
     </row>
@@ -2118,47 +2118,47 @@
         <v xml:space="preserve">MOVE S_CAPS (16.669 47.625); </v>
       </c>
       <c r="C39" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", C32, " (", C25, " ", $Q25,"); ")</f>
+        <f t="shared" ref="C39:M39" si="19">_xlfn.CONCAT("MOVE S_", C32, " (", C25, " ", $Q25,"); ")</f>
         <v xml:space="preserve">MOVE S_A (42.863 47.625); </v>
       </c>
       <c r="D39" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", D32, " (", D25, " ", $Q25,"); ")</f>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">MOVE S_S (61.913 47.625); </v>
       </c>
       <c r="E39" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", E32, " (", E25, " ", $Q25,"); ")</f>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">MOVE S_D (80.963 47.625); </v>
       </c>
       <c r="F39" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", F32, " (", F25, " ", $Q25,"); ")</f>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">MOVE S_F (100.013 47.625); </v>
       </c>
       <c r="G39" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", G32, " (", G25, " ", $Q25,"); ")</f>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">MOVE S_G (119.063 47.625); </v>
       </c>
       <c r="H39" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", H32, " (", H25, " ", $Q25,"); ")</f>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">MOVE S_H (138.113 47.625); </v>
       </c>
       <c r="I39" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", I32, " (", I25, " ", $Q25,"); ")</f>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">MOVE S_J (157.163 47.625); </v>
       </c>
       <c r="J39" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", J32, " (", J25, " ", $Q25,"); ")</f>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">MOVE S_K (176.213 47.625); </v>
       </c>
       <c r="K39" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", K32, " (", K25, " ", $Q25,"); ")</f>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">MOVE S_L (195.263 47.625); </v>
       </c>
       <c r="L39" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", L32, " (", L25, " ", $Q25,"); ")</f>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">MOVE S_SCLN (214.313 47.625); </v>
       </c>
       <c r="M39" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", M32, " (", M25, " ", $Q25,"); ")</f>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">MOVE S_QUOT (233.363 47.625); </v>
       </c>
       <c r="N39" s="4"/>
@@ -2173,43 +2173,43 @@
         <v xml:space="preserve">MOVE S_LSFT (21.431 28.575); </v>
       </c>
       <c r="D40" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", D33, " (", D26, " ", $Q26,"); ")</f>
+        <f t="shared" ref="D40:M40" si="20">_xlfn.CONCAT("MOVE S_", D33, " (", D26, " ", $Q26,"); ")</f>
         <v xml:space="preserve">MOVE S_Z (52.388 28.575); </v>
       </c>
       <c r="E40" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", E33, " (", E26, " ", $Q26,"); ")</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">MOVE S_X (71.438 28.575); </v>
       </c>
       <c r="F40" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", F33, " (", F26, " ", $Q26,"); ")</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">MOVE S_C (90.488 28.575); </v>
       </c>
       <c r="G40" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", G33, " (", G26, " ", $Q26,"); ")</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">MOVE S_V (109.538 28.575); </v>
       </c>
       <c r="H40" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", H33, " (", H26, " ", $Q26,"); ")</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">MOVE S_B (128.588 28.575); </v>
       </c>
       <c r="I40" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", I33, " (", I26, " ", $Q26,"); ")</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">MOVE S_N (147.638 28.575); </v>
       </c>
       <c r="J40" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", J33, " (", J26, " ", $Q26,"); ")</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">MOVE S_M (166.688 28.575); </v>
       </c>
       <c r="K40" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", K33, " (", K26, " ", $Q26,"); ")</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">MOVE S_COM (185.738 28.575); </v>
       </c>
       <c r="L40" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", L33, " (", L26, " ", $Q26,"); ")</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">MOVE S_DOT (204.788 28.575); </v>
       </c>
       <c r="M40" t="str">
-        <f>_xlfn.CONCAT("MOVE S_", M33, " (", M26, " ", $Q26,"); ")</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">MOVE S_SLSH (223.838 28.575); </v>
       </c>
       <c r="N40" s="4"/>
@@ -2288,51 +2288,51 @@
         <v>2</v>
       </c>
       <c r="D46">
-        <f t="shared" ref="D46:O46" si="14">C46+1</f>
+        <f t="shared" ref="D46:O46" si="21">C46+1</f>
         <v>3</v>
       </c>
       <c r="E46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
       <c r="F46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>5</v>
       </c>
       <c r="G46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>6</v>
       </c>
       <c r="H46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
       <c r="I46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>8</v>
       </c>
       <c r="J46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
       <c r="K46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="L46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
       <c r="M46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>12</v>
       </c>
       <c r="N46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>13</v>
       </c>
       <c r="O46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>14</v>
       </c>
     </row>
@@ -2342,55 +2342,55 @@
         <v>15</v>
       </c>
       <c r="C47">
-        <f t="shared" ref="C47:O47" si="15">B47+1</f>
+        <f t="shared" ref="C47:O47" si="22">B47+1</f>
         <v>16</v>
       </c>
       <c r="D47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>17</v>
       </c>
       <c r="E47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>18</v>
       </c>
       <c r="F47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>19</v>
       </c>
       <c r="G47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>20</v>
       </c>
       <c r="H47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>21</v>
       </c>
       <c r="I47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>22</v>
       </c>
       <c r="J47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>23</v>
       </c>
       <c r="K47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>24</v>
       </c>
       <c r="L47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>25</v>
       </c>
       <c r="M47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>26</v>
       </c>
       <c r="N47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>27</v>
       </c>
       <c r="O47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>28</v>
       </c>
     </row>
@@ -2400,47 +2400,47 @@
         <v>29</v>
       </c>
       <c r="C48">
-        <f t="shared" ref="C48:O48" si="16">B48+1</f>
+        <f t="shared" ref="C48:M48" si="23">B48+1</f>
         <v>30</v>
       </c>
       <c r="D48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>31</v>
       </c>
       <c r="E48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>32</v>
       </c>
       <c r="F48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>33</v>
       </c>
       <c r="G48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>34</v>
       </c>
       <c r="H48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>35</v>
       </c>
       <c r="I48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>36</v>
       </c>
       <c r="J48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>37</v>
       </c>
       <c r="K48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>38</v>
       </c>
       <c r="L48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>39</v>
       </c>
       <c r="M48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>40</v>
       </c>
       <c r="O48">
@@ -2458,39 +2458,39 @@
         <v>43</v>
       </c>
       <c r="E49">
-        <f t="shared" ref="C49:O49" si="17">D49+1</f>
+        <f t="shared" ref="E49:M49" si="24">D49+1</f>
         <v>44</v>
       </c>
       <c r="F49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>45</v>
       </c>
       <c r="G49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>46</v>
       </c>
       <c r="H49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>47</v>
       </c>
       <c r="I49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
       <c r="J49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>49</v>
       </c>
       <c r="K49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>50</v>
       </c>
       <c r="L49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>51</v>
       </c>
       <c r="M49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>52</v>
       </c>
       <c r="O49">
@@ -2504,11 +2504,11 @@
         <v>54</v>
       </c>
       <c r="C50">
-        <f t="shared" ref="C50:O50" si="18">B50+1</f>
+        <f t="shared" ref="C50:O50" si="25">B50+1</f>
         <v>55</v>
       </c>
       <c r="D50">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>56</v>
       </c>
       <c r="H50">
@@ -2520,15 +2520,15 @@
         <v>58</v>
       </c>
       <c r="M50">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>59</v>
       </c>
       <c r="N50">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>60</v>
       </c>
       <c r="O50">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>61</v>
       </c>
     </row>
@@ -2549,251 +2549,251 @@
         <v xml:space="preserve">MOVE D1 (3.175 80.675); </v>
       </c>
       <c r="C53" t="str">
-        <f t="shared" ref="C53:O53" si="19">_xlfn.CONCAT("MOVE D", C46, " (", ROUND(INT(C23)+$E$52,3), " ", ROUND(INT($Q23)+$F$52,3),"); ")</f>
+        <f t="shared" ref="C53:O53" si="26">_xlfn.CONCAT("MOVE D", C46, " (", ROUND(INT(C23)+$E$52,3), " ", ROUND(INT($Q23)+$F$52,3),"); ")</f>
         <v xml:space="preserve">MOVE D2 (22.175 80.675); </v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D3 (41.175 80.675); </v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D4 (60.175 80.675); </v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D5 (79.175 80.675); </v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D6 (98.175 80.675); </v>
       </c>
       <c r="H53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D7 (117.175 80.675); </v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D8 (136.175 80.675); </v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D9 (155.175 80.675); </v>
       </c>
       <c r="K53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D10 (174.175 80.675); </v>
       </c>
       <c r="L53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D11 (194.175 80.675); </v>
       </c>
       <c r="M53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D12 (213.175 80.675); </v>
       </c>
       <c r="N53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D13 (232.175 80.675); </v>
       </c>
       <c r="O53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">MOVE D14 (260.175 80.675); </v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B54" t="str">
-        <f t="shared" ref="B54:O54" si="20">_xlfn.CONCAT("MOVE D", B47, " (", ROUND(INT(B24)+$E$52,3), " ", ROUND(INT($Q24)+$F$52,3),"); ")</f>
+        <f t="shared" ref="B54:O54" si="27">_xlfn.CONCAT("MOVE D", B47, " (", ROUND(INT(B24)+$E$52,3), " ", ROUND(INT($Q24)+$F$52,3),"); ")</f>
         <v xml:space="preserve">MOVE D15 (8.175 61.675); </v>
       </c>
       <c r="C54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D16 (32.175 61.675); </v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D17 (51.175 61.675); </v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D18 (70.175 61.675); </v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D19 (89.175 61.675); </v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D20 (108.175 61.675); </v>
       </c>
       <c r="H54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D21 (127.175 61.675); </v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D22 (146.175 61.675); </v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D23 (165.175 61.675); </v>
       </c>
       <c r="K54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D24 (184.175 61.675); </v>
       </c>
       <c r="L54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D25 (203.175 61.675); </v>
       </c>
       <c r="M54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D26 (222.175 61.675); </v>
       </c>
       <c r="N54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D27 (241.175 61.675); </v>
       </c>
       <c r="O54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">MOVE D28 (265.175 61.675); </v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B55" t="str">
-        <f t="shared" ref="B55:O55" si="21">_xlfn.CONCAT("MOVE D", B48, " (", ROUND(INT(B25)+$E$52,3), " ", ROUND(INT($Q25)+$F$52,3),"); ")</f>
+        <f t="shared" ref="B55:O55" si="28">_xlfn.CONCAT("MOVE D", B48, " (", ROUND(INT(B25)+$E$52,3), " ", ROUND(INT($Q25)+$F$52,3),"); ")</f>
         <v xml:space="preserve">MOVE D29 (10.175 42.675); </v>
       </c>
       <c r="C55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D30 (36.175 42.675); </v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D31 (55.175 42.675); </v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D32 (74.175 42.675); </v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D33 (94.175 42.675); </v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D34 (113.175 42.675); </v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D35 (132.175 42.675); </v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D36 (151.175 42.675); </v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D37 (170.175 42.675); </v>
       </c>
       <c r="K55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D38 (189.175 42.675); </v>
       </c>
       <c r="L55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D39 (208.175 42.675); </v>
       </c>
       <c r="M55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D40 (227.175 42.675); </v>
       </c>
       <c r="O55" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">MOVE D41 (258.175 42.675); </v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B56" t="str">
-        <f t="shared" ref="B56:O56" si="22">_xlfn.CONCAT("MOVE D", B49, " (", ROUND(INT(B26)+$E$52,3), " ", ROUND(INT($Q26)+$F$52,3),"); ")</f>
+        <f t="shared" ref="B56:O56" si="29">_xlfn.CONCAT("MOVE D", B49, " (", ROUND(INT(B26)+$E$52,3), " ", ROUND(INT($Q26)+$F$52,3),"); ")</f>
         <v xml:space="preserve">MOVE D42 (15.175 23.675); </v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">MOVE D43 (46.175 23.675); </v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">MOVE D44 (65.175 23.675); </v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">MOVE D45 (84.175 23.675); </v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">MOVE D46 (103.175 23.675); </v>
       </c>
       <c r="H56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">MOVE D47 (122.175 23.675); </v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">MOVE D48 (141.175 23.675); </v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">MOVE D49 (160.175 23.675); </v>
       </c>
       <c r="K56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">MOVE D50 (179.175 23.675); </v>
       </c>
       <c r="L56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">MOVE D51 (198.175 23.675); </v>
       </c>
       <c r="M56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">MOVE D52 (217.175 23.675); </v>
       </c>
       <c r="O56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">MOVE D53 (253.175 23.675); </v>
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B57" t="str">
-        <f t="shared" ref="B57:O57" si="23">_xlfn.CONCAT("MOVE D", B50, " (", ROUND(INT(B27)+$E$52,3), " ", ROUND(INT($Q27)+$F$52,3),"); ")</f>
+        <f t="shared" ref="B57:O57" si="30">_xlfn.CONCAT("MOVE D", B50, " (", ROUND(INT(B27)+$E$52,3), " ", ROUND(INT($Q27)+$F$52,3),"); ")</f>
         <v xml:space="preserve">MOVE D54 (5.175 4.675); </v>
       </c>
       <c r="C57" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v xml:space="preserve">MOVE D55 (29.175 4.675); </v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v xml:space="preserve">MOVE D56 (53.175 4.675); </v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v xml:space="preserve">MOVE D57 (124.175 4.675); </v>
       </c>
       <c r="L57" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v xml:space="preserve">MOVE D58 (196.175 4.675); </v>
       </c>
       <c r="M57" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v xml:space="preserve">MOVE D59 (220.175 4.675); </v>
       </c>
       <c r="N57" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v xml:space="preserve">MOVE D60 (244.175 4.675); </v>
       </c>
       <c r="O57" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v xml:space="preserve">MOVE D61 (267.175 4.675); </v>
       </c>
     </row>

</xml_diff>